<commit_message>
added python script to aggregate results
</commit_message>
<xml_diff>
--- a/Benchmarks/Data/EvaluationData.xlsx
+++ b/Benchmarks/Data/EvaluationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-sumukh\source\repos\p-org\rl\psharp-ql\Benchmarks\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C366F1-CB49-4497-B2F0-A90DF512EB42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8DD2D1-3D69-449A-8759-40EB6CC8C082}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1260" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{69F81732-9917-45FC-B790-578500B02F6D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>Benchmark</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Iterations = 10K, -explore</t>
   </si>
   <si>
-    <t>Iterations = 10K, -explore, -timeout = 5min</t>
-  </si>
-  <si>
     <t>QL-NDN</t>
   </si>
   <si>
@@ -113,13 +110,40 @@
   </si>
   <si>
     <t> 0.0071</t>
+  </si>
+  <si>
+    <t>QL</t>
+  </si>
+  <si>
+    <t>FailureDetector</t>
+  </si>
+  <si>
+    <t>FibBench2</t>
+  </si>
+  <si>
+    <t>FibBenchLongest2</t>
+  </si>
+  <si>
+    <t>Raftv1</t>
+  </si>
+  <si>
+    <t>Raftv2</t>
+  </si>
+  <si>
+    <t>Triangular2</t>
+  </si>
+  <si>
+    <t>TriangularLongest2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Softmax, Iter = 100K, Reset = 1000, -explore, </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,13 +172,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -166,10 +210,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -186,8 +231,11 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>10</v>
@@ -798,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="3">
         <v>0.71319999999999995</v>
@@ -852,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
@@ -934,350 +982,678 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1554B0-8C31-463D-B4D6-5CBEAB732BCA}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>2.3000000000000001E-4</v>
+      </c>
+      <c r="C4">
+        <v>1.7000000000000001E-4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G4">
+        <v>3.5E-4</v>
+      </c>
+      <c r="H4">
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>0.10894</v>
+      </c>
+      <c r="C5">
+        <v>0.10907</v>
+      </c>
+      <c r="D5">
+        <v>4.8689999999999997E-2</v>
+      </c>
+      <c r="E5">
+        <v>3.7920000000000002E-2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>4.2999999999999999E-4</v>
+      </c>
+      <c r="H5">
+        <v>0.70953999999999995</v>
+      </c>
+      <c r="I5">
+        <v>0.95940999999999999</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>6.5740000000000007E-2</v>
+      </c>
+      <c r="C6">
+        <v>1.42E-3</v>
+      </c>
+      <c r="D6">
+        <v>5.1999999999999995E-4</v>
+      </c>
+      <c r="E6">
+        <v>3.65E-3</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I6">
+        <v>0.92291000000000001</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="F7" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="G7">
+        <v>3.3E-4</v>
+      </c>
+      <c r="H7">
+        <v>2.2000000000000001E-4</v>
+      </c>
+      <c r="I7" s="8">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>1.7799999999999999E-3</v>
+      </c>
+      <c r="C8">
+        <v>2.3000000000000001E-4</v>
+      </c>
+      <c r="D8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E8" s="8">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="H8" s="8">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="I8">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>8.3899999999999999E-3</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="E10" s="8">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="I10" s="8">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>1.7330000000000002E-2</v>
+      </c>
+      <c r="C11">
+        <v>1.72E-2</v>
+      </c>
+      <c r="D11">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E11">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1E-4</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="C12">
+        <v>2.2000000000000001E-4</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B16" s="7">
         <v>4.6E-5</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C16" s="7">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
         <v>3.0000000000000001E-6</v>
       </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7">
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="I2" s="3">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B17" s="7">
         <v>5.5000000000000002E-5</v>
       </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D18" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E18" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F18" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G18" s="7">
         <v>7.9999999999999996E-6</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H18" s="7">
         <v>9.0000000000000002E-6</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I18" s="7">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B20" s="7">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C20" s="7">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7">
         <v>1.2E-5</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H20" s="7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B21" s="3">
         <v>7.1349999999999998E-3</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C21" s="3">
         <v>3.3700000000000001E-2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D21" s="3">
         <v>1.5599E-2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E21" s="3">
         <v>1.2264000000000001E-2</v>
       </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
         <v>1.92E-4</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H21" s="3">
         <v>0.17366200000000001</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I21" s="3">
         <v>0.23088800000000001</v>
       </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B22" s="7">
         <v>6.4999999999999994E-5</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C22" s="3">
         <v>1.6069999999999999E-3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D22" s="3">
         <v>1.2899999999999999E-4</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E22" s="3">
         <v>8.3100000000000003E-4</v>
       </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I22" s="3">
         <v>0.13374800000000001</v>
       </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B23" s="7">
         <v>7.3999999999999996E-5</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C23" s="3">
         <v>4.8700000000000002E-3</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D23" s="7">
         <v>6.7000000000000002E-5</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E23" s="3">
         <v>2.0079999999999998E-3</v>
       </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="7">
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I23" s="7">
         <v>3.6000000000000001E-5</v>
       </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="7">
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7">
         <v>3.0000000000000001E-6</v>
       </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7">
         <v>2.8E-5</v>
       </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B25" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E25" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7">
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="7">
         <v>3.0000000000000001E-6</v>
       </c>
-      <c r="J11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
slight fix to computing instabilities
</commit_message>
<xml_diff>
--- a/Benchmarks/Data/EvaluationData.xlsx
+++ b/Benchmarks/Data/EvaluationData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-sumukh\source\repos\p-org\rl\psharp-ql\Benchmarks\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-sumukh\source\repos\p-org\rl-test\psharp-ql\Benchmarks\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850C7ED7-C563-41D3-B66E-C712D7B5E195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F55BF90-7BE0-4A60-BAE7-017C4AB5B3AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{69F81732-9917-45FC-B790-578500B02F6D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{69F81732-9917-45FC-B790-578500B02F6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Random-Timing" sheetId="1" r:id="rId1"/>
-    <sheet name="Protocols-Threading" sheetId="5" r:id="rId2"/>
-    <sheet name="Micro" sheetId="4" r:id="rId3"/>
-    <sheet name="OLD-Protocols-Threading" sheetId="3" r:id="rId4"/>
+    <sheet name="NumericalStability" sheetId="6" r:id="rId2"/>
+    <sheet name="Protocols-Threading" sheetId="5" r:id="rId3"/>
+    <sheet name="Micro" sheetId="4" r:id="rId4"/>
+    <sheet name="OLD-Protocols-Threading" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="41">
   <si>
     <t>Benchmark</t>
   </si>
@@ -242,6 +243,21 @@
   </si>
   <si>
     <t xml:space="preserve">SF = 0.00001, EF = 1,  Iter = 100K, Reset = 10000, -explore, </t>
+  </si>
+  <si>
+    <t>Iter</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>ScaledAvg</t>
+  </si>
+  <si>
+    <t>NaN-Frac</t>
+  </si>
+  <si>
+    <t>B-%</t>
   </si>
 </sst>
 </file>
@@ -328,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -344,6 +360,21 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -662,16 +693,16 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -687,7 +718,7 @@
         <v>197813</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -695,7 +726,7 @@
         <v>181600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -703,7 +734,7 @@
         <v>129619</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -711,7 +742,7 @@
         <v>41610</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -719,7 +750,7 @@
         <v>70940</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -728,7 +759,7 @@
         <v>124316.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -744,6 +775,119 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C2D550-54F6-4467-8D69-C91514156390}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>20000</v>
+      </c>
+      <c r="C3" s="10">
+        <v>5.8179204494309604E-4</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>20000</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>20000</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>20000</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>20000</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5E85FA-3628-45E9-9F29-B5E7B6C4E404}">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -751,12 +895,12 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>35</v>
       </c>
@@ -769,7 +913,7 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -798,7 +942,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -827,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -856,7 +1000,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -885,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -914,7 +1058,7 @@
         <v>0.95945000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -943,7 +1087,7 @@
         <v>0.92310999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -972,7 +1116,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1001,7 +1145,7 @@
         <v>1.6000000000000001E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1030,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1059,7 +1203,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1088,7 +1232,7 @@
         <v>1.8000000000000001E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1123,20 +1267,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1678298-264E-4775-81AC-62F92EC930B1}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.46484375" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>32</v>
       </c>
@@ -1149,7 +1293,7 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1178,7 +1322,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1207,7 +1351,7 @@
         <v>2.7E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>33</v>
       </c>
@@ -1220,7 +1364,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1249,7 +1393,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1278,7 +1422,7 @@
         <v>0.95616000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>34</v>
       </c>
@@ -1291,7 +1435,7 @@
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1320,7 +1464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1355,7 +1499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1554B0-8C31-463D-B4D6-5CBEAB732BCA}">
   <dimension ref="A1:J77"/>
   <sheetViews>
@@ -1363,14 +1507,14 @@
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
@@ -1383,7 +1527,7 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1412,7 +1556,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1441,7 +1585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1470,7 +1614,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1500,7 +1644,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1530,7 +1674,7 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1559,7 +1703,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1588,7 +1732,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1618,7 +1762,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1648,7 +1792,7 @@
       </c>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1678,7 +1822,7 @@
       </c>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1708,10 +1852,10 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>28</v>
       </c>
@@ -1725,7 +1869,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1755,7 +1899,7 @@
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1785,7 +1929,7 @@
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1815,7 +1959,7 @@
       </c>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1845,7 +1989,7 @@
       </c>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1875,7 +2019,7 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1905,7 +2049,7 @@
       </c>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1935,7 +2079,7 @@
       </c>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1965,7 +2109,7 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1994,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2023,7 +2167,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2052,7 +2196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>27</v>
       </c>
@@ -2065,7 +2209,7 @@
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2094,7 +2238,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -2123,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -2152,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -2181,7 +2325,7 @@
         <v>0.83850000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -2210,7 +2354,7 @@
         <v>0.65429999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2239,7 +2383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -2268,7 +2412,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2297,7 +2441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -2326,7 +2470,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2355,7 +2499,7 @@
         <v>1.4999999999999999E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -2384,10 +2528,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>26</v>
       </c>
@@ -2400,7 +2544,7 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2429,7 +2573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -2458,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -2487,7 +2631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -2516,7 +2660,7 @@
         <v>0.83850000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -2545,7 +2689,7 @@
         <v>0.65475000000000005</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -2574,7 +2718,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -2603,7 +2747,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -2632,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -2661,7 +2805,7 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -2690,7 +2834,7 @@
         <v>1.4999999999999999E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -2719,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>25</v>
       </c>
@@ -2732,7 +2876,7 @@
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -2761,7 +2905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
@@ -2790,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>18</v>
       </c>
@@ -2819,7 +2963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>19</v>
       </c>
@@ -2848,7 +2992,7 @@
         <v>0.95940999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>20</v>
       </c>
@@ -2877,7 +3021,7 @@
         <v>0.92291000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>4</v>
       </c>
@@ -2906,7 +3050,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>21</v>
       </c>
@@ -2935,7 +3079,7 @@
         <v>2.4000000000000001E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>22</v>
       </c>
@@ -2964,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>15</v>
       </c>
@@ -2993,7 +3137,7 @@
         <v>6.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>23</v>
       </c>
@@ -3022,7 +3166,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>24</v>
       </c>
@@ -3051,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -3062,7 +3206,7 @@
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -3073,7 +3217,7 @@
       <c r="H68" s="6"/>
       <c r="I68" s="3"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="C69" s="3"/>
@@ -3084,7 +3228,7 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="3"/>
       <c r="C70" s="6"/>
@@ -3095,7 +3239,7 @@
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -3106,7 +3250,7 @@
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -3117,7 +3261,7 @@
       <c r="H72" s="6"/>
       <c r="I72" s="3"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -3128,7 +3272,7 @@
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="6"/>
       <c r="C74" s="3"/>
@@ -3139,7 +3283,7 @@
       <c r="H74" s="6"/>
       <c r="I74" s="3"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="6"/>
       <c r="C75" s="3"/>
@@ -3150,7 +3294,7 @@
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="3"/>
       <c r="C76" s="6"/>
@@ -3161,7 +3305,7 @@
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="6"/>
       <c r="C77" s="3"/>

</xml_diff>